<commit_message>
add data issues col (e.g. sum vs. avg)
</commit_message>
<xml_diff>
--- a/US/lead_data/reuters/description-of-raw-BLL-data.xlsx
+++ b/US/lead_data/reuters/description-of-raw-BLL-data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27809"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xilin/Documents/GitHub/leadmap-public/reuters/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lasse/Library/Mobile Documents/com~apple~CloudDocs/Oxford MPhil/GRA Frank/lead_map/US/lead_data/reuters/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF282CF0-98E2-2E4A-B8BC-5BEEAF8747F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="500" windowWidth="25500" windowHeight="19320" tabRatio="500"/>
+    <workbookView xWindow="1280" yWindow="760" windowWidth="25500" windowHeight="18880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="87">
   <si>
     <t>State</t>
   </si>
@@ -279,16 +280,35 @@
   </si>
   <si>
     <t>Potential Problems</t>
+  </si>
+  <si>
+    <t>AVERAGE VS SUM?</t>
+  </si>
+  <si>
+    <t>Separate Test numbers for different exposure classes</t>
+  </si>
+  <si>
+    <t>confirmed vs. Estimated</t>
+  </si>
+  <si>
+    <t>Data Issues</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -320,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -332,11 +352,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -346,6 +362,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -613,11 +632,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -628,7 +647,7 @@
     <col min="8" max="8" width="65" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>82</v>
       </c>
@@ -653,8 +672,11 @@
       <c r="H1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
@@ -674,7 +696,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>15</v>
       </c>
@@ -694,7 +716,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>24</v>
       </c>
@@ -717,7 +739,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>25</v>
       </c>
@@ -739,8 +761,11 @@
       <c r="H5" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>29</v>
       </c>
@@ -760,7 +785,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>31</v>
       </c>
@@ -780,7 +805,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>34</v>
       </c>
@@ -800,27 +825,27 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="7" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>38</v>
       </c>
@@ -840,7 +865,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
         <v>42</v>
       </c>
@@ -863,30 +888,33 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="B12" s="5" t="s">
+    <row r="12" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H12" s="6" t="s">
+      <c r="E12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" s="3" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="I12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>80</v>
       </c>
@@ -912,7 +940,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
         <v>46</v>
       </c>
@@ -932,7 +960,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>81</v>
       </c>
@@ -954,8 +982,11 @@
       <c r="G15" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>49</v>
       </c>
@@ -978,7 +1009,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>51</v>
       </c>
@@ -1000,8 +1031,11 @@
       <c r="H17" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
         <v>52</v>
       </c>
@@ -1021,7 +1055,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>54</v>
       </c>
@@ -1041,7 +1075,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="3" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" s="3" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>80</v>
       </c>
@@ -1067,7 +1101,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B21" s="3" t="s">
         <v>57</v>
       </c>
@@ -1087,7 +1121,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>58</v>
       </c>
@@ -1107,7 +1141,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="3" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>79</v>
       </c>
@@ -1133,7 +1167,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="3" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="B24" s="3" t="s">
         <v>61</v>
       </c>
@@ -1156,7 +1190,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="3" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="B25" s="3" t="s">
         <v>62</v>
       </c>
@@ -1179,7 +1213,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>63</v>
       </c>
@@ -1202,7 +1236,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="3" t="s">
         <v>65</v>
       </c>
@@ -1222,7 +1256,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="3" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>79</v>
       </c>
@@ -1248,7 +1282,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B29" s="3" t="s">
         <v>67</v>
       </c>
@@ -1268,7 +1302,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>69</v>
       </c>
@@ -1291,7 +1325,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B31" s="2" t="s">
         <v>72</v>
       </c>
@@ -1313,8 +1347,11 @@
       <c r="H31" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I31" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>73</v>
       </c>
@@ -1322,7 +1359,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="2:8" s="3" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:9" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="B33" s="3" t="s">
         <v>75</v>
       </c>
@@ -1345,7 +1382,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B34" s="2" t="s">
         <v>76</v>
       </c>
@@ -1368,7 +1405,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>77</v>
       </c>
@@ -1387,8 +1424,11 @@
       <c r="G35" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I35" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>78</v>
       </c>

</xml_diff>

<commit_message>
rm TODO for wisconsin
</commit_message>
<xml_diff>
--- a/US/lead_data/reuters/description-of-raw-BLL-data.xlsx
+++ b/US/lead_data/reuters/description-of-raw-BLL-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lasse/Library/Mobile Documents/com~apple~CloudDocs/Oxford MPhil/GRA Frank/lead_map/US/lead_data/reuters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0061FB01-62E7-D04C-8213-2D16CCDEABAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC7E6001-778A-D64D-9772-FFF1B1209BB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="760" windowWidth="29260" windowHeight="18880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="103">
   <si>
     <t>State</t>
   </si>
@@ -748,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1825,9 +1825,7 @@
       <c r="J36" s="1"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>99</v>
-      </c>
+      <c r="A37" s="1"/>
       <c r="B37" s="1" t="s">
         <v>71</v>
       </c>

</xml_diff>